<commit_message>
improve cell segmentation algorithm. use histogram for identifying cells with no inclusions
</commit_message>
<xml_diff>
--- a/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
+++ b/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C166"/>
+  <dimension ref="A1:C160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,20 +466,20 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_03</t>
+          <t>1K_ADAMTS19_01</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_04</t>
+          <t>1K_ADAMTS19_02</t>
         </is>
       </c>
       <c r="B4" t="n">
@@ -492,37 +492,37 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_04</t>
+          <t>1K_ADAMTS19_03</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_05</t>
+          <t>1K_ADAMTS19_03</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_05</t>
+          <t>1K_ADAMTS19_03</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
@@ -531,11 +531,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_05</t>
+          <t>1K_ADAMTS19_03</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
@@ -544,33 +544,33 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_05</t>
+          <t>1K_ADAMTS19_04</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_05</t>
+          <t>1K_ADAMTS19_04</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_06</t>
+          <t>1K_ADAMTS19_05</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -583,11 +583,11 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_07</t>
+          <t>1K_ADAMTS19_05</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
@@ -596,11 +596,11 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_07</t>
+          <t>1K_ADAMTS19_06</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
@@ -609,7 +609,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_08</t>
+          <t>1K_ADAMTS19_07</t>
         </is>
       </c>
       <c r="B14" t="n">
@@ -622,7 +622,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_08</t>
+          <t>1K_ADAMTS19_07</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -635,7 +635,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_08</t>
+          <t>1K_ADAMTS19_07</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -648,7 +648,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_09</t>
+          <t>1K_ADAMTS19_08</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -661,7 +661,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_09</t>
+          <t>1K_ADAMTS19_08</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -678,7 +678,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
@@ -691,7 +691,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
@@ -704,7 +704,7 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
@@ -713,11 +713,11 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_09</t>
+          <t>1K_ADAMTS19_10</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
@@ -726,14 +726,14 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_09</t>
+          <t>1K_ADAMTS19_10</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
@@ -743,23 +743,23 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>1K_ADAMTS19_10</t>
+          <t>1K_SCR_01</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C25" t="n">
-        <v>7</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C26" t="n">
-        <v>17</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27">
@@ -782,20 +782,20 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>1K_SCR_01</t>
+          <t>1K_SCR_02</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
@@ -808,7 +808,7 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
@@ -817,11 +817,11 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>1K_SCR_02</t>
+          <t>1K_SCR_03</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
@@ -830,24 +830,24 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>1K_SCR_02</t>
+          <t>1K_SCR_03</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>1K_SCR_02</t>
+          <t>1K_SCR_04</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
@@ -856,11 +856,11 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>1K_SCR_03</t>
+          <t>1K_SCR_04</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
@@ -869,14 +869,14 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>1K_SCR_03</t>
+          <t>1K_SCR_04</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
@@ -886,7 +886,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
@@ -908,14 +908,14 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>1K_SCR_04</t>
+          <t>1K_SCR_05</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C38" t="n">
         <v>1</v>
@@ -938,20 +938,20 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C39" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>1K_SCR_05</t>
+          <t>1K_SCR_06</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
@@ -964,7 +964,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
@@ -977,7 +977,7 @@
         </is>
       </c>
       <c r="B42" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
@@ -990,7 +990,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
@@ -1003,7 +1003,7 @@
         </is>
       </c>
       <c r="B44" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
@@ -1016,7 +1016,7 @@
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
@@ -1129,11 +1129,11 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>1K_SCR_08</t>
+          <t>1K_SCR_09</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
@@ -1146,7 +1146,7 @@
         </is>
       </c>
       <c r="B55" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
@@ -1159,7 +1159,7 @@
         </is>
       </c>
       <c r="B56" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
@@ -1168,11 +1168,11 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>1K_SCR_09</t>
+          <t>1K_SCR_10</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
@@ -1181,11 +1181,11 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>1K_SCR_09</t>
+          <t>1K_SCR_10</t>
         </is>
       </c>
       <c r="B58" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
@@ -1194,11 +1194,11 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>1K_SCR_09</t>
+          <t>1K_SCR_10</t>
         </is>
       </c>
       <c r="B59" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
@@ -1207,37 +1207,37 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>1K_SCR_10</t>
+          <t>1K_TAX1BP1_01</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>0</v>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>1K_SCR_10</t>
+          <t>1K_TAX1BP1_02</t>
         </is>
       </c>
       <c r="B61" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C61" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>1K_SCR_10</t>
+          <t>1K_TAX1BP1_04</t>
         </is>
       </c>
       <c r="B62" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
@@ -1246,40 +1246,40 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_01</t>
+          <t>1K_TAX1BP1_04</t>
         </is>
       </c>
       <c r="B63" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_02</t>
+          <t>1K_TAX1BP1_05</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>0</v>
       </c>
       <c r="C64" t="n">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_04</t>
+          <t>1K_TAX1BP1_05</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C65" t="n">
-        <v>17</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -1289,7 +1289,7 @@
         </is>
       </c>
       <c r="B66" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
@@ -1298,11 +1298,11 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_05</t>
+          <t>1K_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B67" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
@@ -1315,7 +1315,7 @@
         </is>
       </c>
       <c r="B68" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
@@ -1328,7 +1328,7 @@
         </is>
       </c>
       <c r="B69" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
@@ -1337,37 +1337,37 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_06</t>
+          <t>1K_TAX1BP1_07</t>
         </is>
       </c>
       <c r="B70" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C70" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_10</t>
+          <t>1K_TAX1BP1_08</t>
         </is>
       </c>
       <c r="B71" t="n">
         <v>0</v>
       </c>
       <c r="C71" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_10</t>
+          <t>1K_TAX1BP1_09</t>
         </is>
       </c>
       <c r="B72" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C72" t="n">
         <v>1</v>
@@ -1380,7 +1380,7 @@
         </is>
       </c>
       <c r="B73" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C73" t="n">
         <v>0</v>
@@ -1393,10 +1393,10 @@
         </is>
       </c>
       <c r="B74" t="n">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
@@ -1406,7 +1406,7 @@
         </is>
       </c>
       <c r="B75" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C75" t="n">
         <v>0</v>
@@ -1415,14 +1415,14 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>1K_TAX1BP1_10</t>
+          <t>WT_ADAMTS19_01</t>
         </is>
       </c>
       <c r="B76" t="n">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
@@ -1558,11 +1558,11 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_04</t>
+          <t>WT_ADAMTS19_05</t>
         </is>
       </c>
       <c r="B87" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C87" t="n">
         <v>0</v>
@@ -1575,7 +1575,7 @@
         </is>
       </c>
       <c r="B88" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C88" t="n">
         <v>0</v>
@@ -1588,7 +1588,7 @@
         </is>
       </c>
       <c r="B89" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C89" t="n">
         <v>0</v>
@@ -1597,11 +1597,11 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_05</t>
+          <t>WT_ADAMTS19_06</t>
         </is>
       </c>
       <c r="B90" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C90" t="n">
         <v>0</v>
@@ -1614,7 +1614,7 @@
         </is>
       </c>
       <c r="B91" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C91" t="n">
         <v>0</v>
@@ -1627,7 +1627,7 @@
         </is>
       </c>
       <c r="B92" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C92" t="n">
         <v>0</v>
@@ -1640,7 +1640,7 @@
         </is>
       </c>
       <c r="B93" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C93" t="n">
         <v>0</v>
@@ -1649,24 +1649,24 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_06</t>
+          <t>WT_ADAMTS19_07</t>
         </is>
       </c>
       <c r="B94" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_06</t>
+          <t>WT_ADAMTS19_07</t>
         </is>
       </c>
       <c r="B95" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C95" t="n">
         <v>0</v>
@@ -1675,20 +1675,20 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_07</t>
+          <t>WT_ADAMTS19_08</t>
         </is>
       </c>
       <c r="B96" t="n">
         <v>0</v>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_07</t>
+          <t>WT_ADAMTS19_08</t>
         </is>
       </c>
       <c r="B97" t="n">
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="B98" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C98" t="n">
         <v>0</v>
@@ -1714,11 +1714,11 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_08</t>
+          <t>WT_ADAMTS19_09</t>
         </is>
       </c>
       <c r="B99" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C99" t="n">
         <v>0</v>
@@ -1727,11 +1727,11 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_08</t>
+          <t>WT_ADAMTS19_09</t>
         </is>
       </c>
       <c r="B100" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C100" t="n">
         <v>0</v>
@@ -1740,11 +1740,11 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_08</t>
+          <t>WT_ADAMTS19_09</t>
         </is>
       </c>
       <c r="B101" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C101" t="n">
         <v>0</v>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="B102" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C102" t="n">
         <v>0</v>
@@ -1766,24 +1766,24 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_09</t>
+          <t>WT_ADAMTS19_10</t>
         </is>
       </c>
       <c r="B103" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_09</t>
+          <t>WT_SCR_01</t>
         </is>
       </c>
       <c r="B104" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C104" t="n">
         <v>0</v>
@@ -1792,24 +1792,24 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_09</t>
+          <t>WT_SCR_01</t>
         </is>
       </c>
       <c r="B105" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_09</t>
+          <t>WT_SCR_01</t>
         </is>
       </c>
       <c r="B106" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C106" t="n">
         <v>0</v>
@@ -1818,7 +1818,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>WT_ADAMTS19_10</t>
+          <t>WT_SCR_02</t>
         </is>
       </c>
       <c r="B107" t="n">
@@ -1831,11 +1831,11 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>WT_SCR_01</t>
+          <t>WT_SCR_02</t>
         </is>
       </c>
       <c r="B108" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C108" t="n">
         <v>0</v>
@@ -1844,11 +1844,11 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>WT_SCR_01</t>
+          <t>WT_SCR_02</t>
         </is>
       </c>
       <c r="B109" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C109" t="n">
         <v>0</v>
@@ -1861,7 +1861,7 @@
         </is>
       </c>
       <c r="B110" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
@@ -1870,24 +1870,24 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>WT_SCR_02</t>
+          <t>WT_SCR_03</t>
         </is>
       </c>
       <c r="B111" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>WT_SCR_02</t>
+          <t>WT_SCR_04</t>
         </is>
       </c>
       <c r="B112" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C112" t="n">
         <v>0</v>
@@ -1896,11 +1896,11 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>WT_SCR_02</t>
+          <t>WT_SCR_04</t>
         </is>
       </c>
       <c r="B113" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C113" t="n">
         <v>0</v>
@@ -1909,11 +1909,11 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>WT_SCR_03</t>
+          <t>WT_SCR_04</t>
         </is>
       </c>
       <c r="B114" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
@@ -1922,24 +1922,24 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>WT_SCR_03</t>
+          <t>WT_SCR_05</t>
         </is>
       </c>
       <c r="B115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C115" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>WT_SCR_04</t>
+          <t>WT_SCR_05</t>
         </is>
       </c>
       <c r="B116" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C116" t="n">
         <v>0</v>
@@ -1948,11 +1948,11 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>WT_SCR_04</t>
+          <t>WT_SCR_06</t>
         </is>
       </c>
       <c r="B117" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
@@ -1961,11 +1961,11 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>WT_SCR_04</t>
+          <t>WT_SCR_06</t>
         </is>
       </c>
       <c r="B118" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
@@ -1974,24 +1974,24 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>WT_SCR_05</t>
+          <t>WT_SCR_06</t>
         </is>
       </c>
       <c r="B119" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C119" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>WT_SCR_05</t>
+          <t>WT_SCR_07</t>
         </is>
       </c>
       <c r="B120" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C120" t="n">
         <v>0</v>
@@ -2000,37 +2000,37 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>WT_SCR_05</t>
+          <t>WT_SCR_07</t>
         </is>
       </c>
       <c r="B121" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C121" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>WT_SCR_05</t>
+          <t>WT_SCR_08</t>
         </is>
       </c>
       <c r="B122" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C122" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>WT_SCR_06</t>
+          <t>WT_SCR_08</t>
         </is>
       </c>
       <c r="B123" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
@@ -2039,24 +2039,24 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>WT_SCR_06</t>
+          <t>WT_SCR_08</t>
         </is>
       </c>
       <c r="B124" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C124" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>WT_SCR_06</t>
+          <t>WT_SCR_08</t>
         </is>
       </c>
       <c r="B125" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
@@ -2065,11 +2065,11 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>WT_SCR_06</t>
+          <t>WT_SCR_08</t>
         </is>
       </c>
       <c r="B126" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
@@ -2078,7 +2078,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>WT_SCR_07</t>
+          <t>WT_SCR_09</t>
         </is>
       </c>
       <c r="B127" t="n">
@@ -2091,7 +2091,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>WT_SCR_07</t>
+          <t>WT_SCR_09</t>
         </is>
       </c>
       <c r="B128" t="n">
@@ -2104,11 +2104,11 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>WT_SCR_07</t>
+          <t>WT_SCR_10</t>
         </is>
       </c>
       <c r="B129" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -2117,11 +2117,11 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>WT_SCR_07</t>
+          <t>WT_SCR_10</t>
         </is>
       </c>
       <c r="B130" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C130" t="n">
         <v>1</v>
@@ -2130,24 +2130,24 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>WT_SCR_08</t>
+          <t>WT_SCR_10</t>
         </is>
       </c>
       <c r="B131" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>WT_SCR_08</t>
+          <t>WT_TAX1BP1_01</t>
         </is>
       </c>
       <c r="B132" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C132" t="n">
         <v>0</v>
@@ -2156,24 +2156,24 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>WT_SCR_08</t>
+          <t>WT_TAX1BP1_01</t>
         </is>
       </c>
       <c r="B133" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C133" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>WT_SCR_08</t>
+          <t>WT_TAX1BP1_01</t>
         </is>
       </c>
       <c r="B134" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C134" t="n">
         <v>0</v>
@@ -2182,20 +2182,20 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>WT_SCR_08</t>
+          <t>WT_TAX1BP1_01</t>
         </is>
       </c>
       <c r="B135" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>WT_SCR_09</t>
+          <t>WT_TAX1BP1_02</t>
         </is>
       </c>
       <c r="B136" t="n">
@@ -2208,7 +2208,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>WT_SCR_09</t>
+          <t>WT_TAX1BP1_02</t>
         </is>
       </c>
       <c r="B137" t="n">
@@ -2221,11 +2221,11 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>WT_SCR_10</t>
+          <t>WT_TAX1BP1_02</t>
         </is>
       </c>
       <c r="B138" t="n">
-        <v>33</v>
+        <v>2</v>
       </c>
       <c r="C138" t="n">
         <v>0</v>
@@ -2234,33 +2234,33 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>WT_SCR_10</t>
+          <t>WT_TAX1BP1_02</t>
         </is>
       </c>
       <c r="B139" t="n">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="C139" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_01</t>
+          <t>WT_TAX1BP1_03</t>
         </is>
       </c>
       <c r="B140" t="n">
         <v>0</v>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_01</t>
+          <t>WT_TAX1BP1_03</t>
         </is>
       </c>
       <c r="B141" t="n">
@@ -2273,50 +2273,50 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_01</t>
+          <t>WT_TAX1BP1_03</t>
         </is>
       </c>
       <c r="B142" t="n">
         <v>2</v>
       </c>
       <c r="C142" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_02</t>
+          <t>WT_TAX1BP1_04</t>
         </is>
       </c>
       <c r="B143" t="n">
         <v>0</v>
       </c>
       <c r="C143" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_02</t>
+          <t>WT_TAX1BP1_04</t>
         </is>
       </c>
       <c r="B144" t="n">
         <v>1</v>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_02</t>
+          <t>WT_TAX1BP1_05</t>
         </is>
       </c>
       <c r="B145" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C145" t="n">
         <v>1</v>
@@ -2325,24 +2325,24 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_03</t>
+          <t>WT_TAX1BP1_05</t>
         </is>
       </c>
       <c r="B146" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C146" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_03</t>
+          <t>WT_TAX1BP1_05</t>
         </is>
       </c>
       <c r="B147" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147" t="n">
         <v>0</v>
@@ -2351,50 +2351,50 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_03</t>
+          <t>WT_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B148" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C148" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_04</t>
+          <t>WT_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B149" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C149" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_05</t>
+          <t>WT_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C150" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_05</t>
+          <t>WT_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B151" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C151" t="n">
         <v>0</v>
@@ -2403,33 +2403,33 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_05</t>
+          <t>WT_TAX1BP1_06</t>
         </is>
       </c>
       <c r="B152" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C152" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_05</t>
+          <t>WT_TAX1BP1_07</t>
         </is>
       </c>
       <c r="B153" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_06</t>
+          <t>WT_TAX1BP1_08</t>
         </is>
       </c>
       <c r="B154" t="n">
@@ -2442,7 +2442,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_06</t>
+          <t>WT_TAX1BP1_08</t>
         </is>
       </c>
       <c r="B155" t="n">
@@ -2455,144 +2455,66 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_06</t>
+          <t>WT_TAX1BP1_08</t>
         </is>
       </c>
       <c r="B156" t="n">
         <v>2</v>
       </c>
       <c r="C156" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_06</t>
+          <t>WT_TAX1BP1_09</t>
         </is>
       </c>
       <c r="B157" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_06</t>
+          <t>WT_TAX1BP1_10</t>
         </is>
       </c>
       <c r="B158" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C158" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_07</t>
+          <t>WT_TAX1BP1_10</t>
         </is>
       </c>
       <c r="B159" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C159" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>WT_TAX1BP1_08</t>
+          <t>WT_TAX1BP1_10</t>
         </is>
       </c>
       <c r="B160" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_08</t>
-        </is>
-      </c>
-      <c r="B161" t="n">
-        <v>1</v>
-      </c>
-      <c r="C161" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_08</t>
-        </is>
-      </c>
-      <c r="B162" t="n">
-        <v>2</v>
-      </c>
-      <c r="C162" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_08</t>
-        </is>
-      </c>
-      <c r="B163" t="n">
-        <v>3</v>
-      </c>
-      <c r="C163" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164">
-      <c r="A164" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_09</t>
-        </is>
-      </c>
-      <c r="B164" t="n">
-        <v>0</v>
-      </c>
-      <c r="C164" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="165">
-      <c r="A165" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_10</t>
-        </is>
-      </c>
-      <c r="B165" t="n">
-        <v>0</v>
-      </c>
-      <c r="C165" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166">
-      <c r="A166" t="inlineStr">
-        <is>
-          <t>WT_TAX1BP1_10</t>
-        </is>
-      </c>
-      <c r="B166" t="n">
-        <v>1</v>
-      </c>
-      <c r="C166" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use 3rd quartile instead of mean
</commit_message>
<xml_diff>
--- a/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
+++ b/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
@@ -473,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -499,7 +499,7 @@
         <v>2</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
@@ -980,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43">
@@ -1019,7 +1019,7 @@
         <v>2</v>
       </c>
       <c r="C45" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="73">
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="74">
@@ -1396,7 +1396,7 @@
         <v>0</v>
       </c>
       <c r="C74" t="n">
-        <v>37</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75">
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
@@ -1916,7 +1916,7 @@
         <v>0</v>
       </c>
       <c r="C114" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
@@ -2059,7 +2059,7 @@
         <v>0</v>
       </c>
       <c r="C125" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="126">
@@ -2384,7 +2384,7 @@
         <v>0</v>
       </c>
       <c r="C150" t="n">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151">
@@ -2878,7 +2878,7 @@
         <v>4</v>
       </c>
       <c r="C188" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">

</xml_diff>

<commit_message>
analyze 120524 and improve algorithm
</commit_message>
<xml_diff>
--- a/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
+++ b/PFF_SCR_TAX_ADAM/011124_analysis_by_cell_NEW.xlsx
@@ -850,7 +850,7 @@
         <v>0</v>
       </c>
       <c r="C32" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
     </row>
     <row r="33">
@@ -876,7 +876,7 @@
         <v>0</v>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35">
@@ -980,7 +980,7 @@
         <v>1</v>
       </c>
       <c r="C42" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
       <c r="C72" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
@@ -1383,7 +1383,7 @@
         <v>0</v>
       </c>
       <c r="C73" t="n">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="74">
@@ -1526,7 +1526,7 @@
         <v>0</v>
       </c>
       <c r="C84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
@@ -1643,7 +1643,7 @@
         <v>0</v>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="94">
@@ -1669,7 +1669,7 @@
         <v>1</v>
       </c>
       <c r="C95" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -2709,7 +2709,7 @@
         <v>0</v>
       </c>
       <c r="C175" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="176">

</xml_diff>